<commit_message>
Centro de notificaciones terminado
</commit_message>
<xml_diff>
--- a/Hardware/EstacionTerrena/BOM.xlsx
+++ b/Hardware/EstacionTerrena/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git-Repos\CanSat\Hardware\EstacionTerrena\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\Repos\CanSat\Hardware\EstacionTerrena\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EstacionTerrena_" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>5-1814832-1</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>Generic connector, single row, 01x03, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>100pF</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -672,26 +672,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.3046875" customWidth="1"/>
-    <col min="2" max="2" width="42.765625" customWidth="1"/>
-    <col min="3" max="3" width="18.61328125" customWidth="1"/>
-    <col min="4" max="4" width="24.23046875" customWidth="1"/>
-    <col min="5" max="5" width="18.61328125" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="22.84375" customWidth="1"/>
-    <col min="9" max="1025" width="11.53515625"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -742,8 +742,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -769,7 +772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -780,10 +783,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
         <v>107</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -794,8 +797,11 @@
       <c r="H4" s="2">
         <v>885012005046</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -820,8 +826,11 @@
       <c r="H5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -847,7 +856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -872,8 +881,11 @@
       <c r="H7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -898,8 +910,11 @@
       <c r="H8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -924,8 +939,11 @@
       <c r="H9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -936,7 +954,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -950,25 +968,28 @@
       <c r="H10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
         <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -977,365 +998,395 @@
         <v>61300311121</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
         <v>45</v>
       </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
         <v>46</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
         <v>50</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>55</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
         <v>56</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>60</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>61</v>
-      </c>
-      <c r="F15" t="s">
-        <v>62</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
       <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
         <v>64</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>65</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>66</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17">
         <v>220</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
       <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
         <v>71</v>
       </c>
-      <c r="F18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" t="s">
-        <v>75</v>
-      </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" t="s">
         <v>78</v>
       </c>
-      <c r="E20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" t="s">
-        <v>79</v>
-      </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
         <v>80</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" t="s">
         <v>82</v>
       </c>
-      <c r="E21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
         <v>83</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>86</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" t="s">
         <v>87</v>
       </c>
-      <c r="E22" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>88</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
         <v>92</v>
       </c>
-      <c r="E23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
         <v>93</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>96</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>97</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>98</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
         <v>99</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
         <v>101</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>102</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>103</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>104</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
         <v>105</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>106</v>
+      <c r="I25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>